<commit_message>
Several pernicious bug fixes.
</commit_message>
<xml_diff>
--- a/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Simulation_From_Motor_Neuron_Activations/debugging_check_list.xlsx
+++ b/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Simulation_From_Motor_Neuron_Activations/debugging_check_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Quadruped_Robot\Code\Matlab\Quadruped_Simulation\Quadruped_Simulation_Framework\Main\Simulation\Software\Simulation_From_Motor_Neuron_Activations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B27685-2759-40A2-AE6D-0CE051119446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8D0CE3-1788-423D-BFC9-20668B2D8A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37C4A111-7CC5-42FE-878D-88FD8D510F88}"/>
   </bookViews>
@@ -312,8 +312,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -347,10 +355,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,11 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EA077A-DA77-48D7-B39B-3510DF96090C}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,58 +709,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="2" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="3" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" t="s">
         <v>51</v>
       </c>
@@ -788,8 +797,8 @@
       <c r="N3" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -857,7 +866,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>A5+1</f>
+        <f t="shared" ref="A6:A14" si="0">A5+1</f>
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -893,7 +902,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B7" t="s">
@@ -908,7 +917,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B8" t="s">
@@ -920,13 +929,13 @@
       <c r="D8" t="s">
         <v>61</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="7" t="s">
         <v>74</v>
       </c>
       <c r="K8" t="s">
@@ -938,7 +947,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B9" t="s">
@@ -968,7 +977,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B10" t="s">
@@ -1004,13 +1013,13 @@
       <c r="L10" t="s">
         <v>84</v>
       </c>
-      <c r="X10" s="4" t="s">
+      <c r="X10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B11" t="s">
@@ -1031,7 +1040,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B12" t="s">
@@ -1064,7 +1073,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B13" t="s">
@@ -1079,7 +1088,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B14" t="s">
@@ -1106,7 +1115,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" ref="A15:A17" si="0">A14+1</f>
+        <f t="shared" ref="A15:A17" si="1">A14+1</f>
         <v>11</v>
       </c>
       <c r="B15" t="s">
@@ -1130,7 +1139,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B16" t="s">
@@ -1148,7 +1157,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B17" t="s">
@@ -1175,6 +1184,7 @@
     <mergeCell ref="P2:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1189,69 +1199,69 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="2" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" t="s">
         <v>14</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1298,14 +1308,14 @@
       <c r="H6" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -1316,35 +1326,35 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
@@ -1358,7 +1368,7 @@
       <c r="H14" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1366,10 +1376,10 @@
       <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1431,12 +1441,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:P3"/>
-    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Attempting to fix conflict.
</commit_message>
<xml_diff>
--- a/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Simulation_From_Motor_Neuron_Activations/debugging_check_list.xlsx
+++ b/Code/Matlab/Quadruped_Simulation/Quadruped_Simulation_Framework/Main/Simulation/Software/Simulation_From_Motor_Neuron_Activations/debugging_check_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Quadruped_Robot\Code\Matlab\Quadruped_Simulation\Quadruped_Simulation_Framework\Main\Simulation\Software\Simulation_From_Motor_Neuron_Activations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8D0CE3-1788-423D-BFC9-20668B2D8A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4A27A9-7A7E-418F-BB4C-D4E321437871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37C4A111-7CC5-42FE-878D-88FD8D510F88}"/>
   </bookViews>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EA077A-DA77-48D7-B39B-3510DF96090C}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>